<commit_message>
major improvements, use api instead of frontend
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brock\Desktop\Mercedes Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE32E73D-C137-4546-99CB-37460F48721E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4A327F-189A-49CD-A435-F5FF1F201940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1752" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="2736" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -361,7 +361,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G24"/>
+      <selection sqref="A1:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
organization + backend improvements
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brock\Desktop\Mercedes Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4A327F-189A-49CD-A435-F5FF1F201940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B06C890-D5BF-4A05-A852-4D1858E9BA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="2736" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,11 +360,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
change sorting algo to stable to preserve order
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brock\Desktop\Mercedes Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B06C890-D5BF-4A05-A852-4D1858E9BA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25629F9-DC7E-4C32-9E16-59E6E5089F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,8 +360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>